<commit_message>
RDM-13008 Add role-to-access-profiles to CCD_BEFTA_JURISDICTION1.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semenu/projects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4325C90D-0404-534C-98C4-4DD9FE1DAF2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{80281D42-E6D3-499C-90C4-C2B297A7FCE6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56307C8C-DDC2-FF48-81D2-76F3B61DA6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" tabRatio="823" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,11 +32,12 @@
     <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId17"/>
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
+    <sheet name="RoleToAccessProfiles" sheetId="20" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="215">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -658,18 +659,79 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>Case Type Id</t>
+  </si>
+  <si>
+    <t>Access Profiles</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>Role1</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Role2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ROLE_TO_ACCESS_PROFILE_CASE_TYPE</t>
+  </si>
+  <si>
+    <t>For testing role to access profile case type</t>
+  </si>
+  <si>
+    <t>RTAP_CASE_TYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="d&quot;/&quot;m&quot;/&quot;yy"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -948,8 +1010,43 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -974,8 +1071,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1037,8 +1140,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1068,8 +1232,9 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1185,8 +1350,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="28" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="29" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="29" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="29"/>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="5" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="5" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="5" borderId="5" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="29" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="5" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="0" borderId="5" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="29" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="6" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="0" borderId="7" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="8" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="8" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="9" xfId="29" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
@@ -1216,8 +1446,335 @@
     <cellStyle name="Normal 2 3" xfId="25" xr:uid="{B75572D7-6A12-2E4F-BFA2-198FB3AC3812}"/>
     <cellStyle name="Normal 3" xfId="26" xr:uid="{63780BEC-AE4D-934E-9473-A01E2AF084BD}"/>
     <cellStyle name="Normal 3 2" xfId="27" xr:uid="{1FA08255-7C4C-8944-85A6-8E22F65BB926}"/>
+    <cellStyle name="Normal 4" xfId="29" xr:uid="{B6EE3D79-7C13-9143-8C0F-9938491FDAB6}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1241,6 +1798,22 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB777435-0AD8-EA4C-A4EE-C9BE1C5AD595}" name="Table2214" displayName="Table2214" ref="A3:H58" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9572B57F-38EA-A146-806B-BFD81A8F93B0}" name="LiveFrom" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{6B9FC0EC-B825-254E-B887-2D066A95169C}" name="LiveTo" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{38068886-0FC7-094A-82DA-0C574E544D5A}" name="RoleName" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{8DF5B2A6-270E-B84B-9C39-5B60D3AADB05}" name="Authorisation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3F993487-9D66-B440-A077-61000424DED7}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E26F0235-B7B7-B140-A113-B2BEA3AFE327}" name="AccessProfiles" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7DEB4409-E2B8-3E41-8AE5-274AA577F558}" name="ReadOnly" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C4E4EFF7-0792-F049-8585-D89766580AAA}" name="Disabled" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1536,16 +2109,16 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +2133,7 @@
       </c>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
@@ -1573,7 +2146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1590,7 +2163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -1626,23 +2199,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -1658,7 +2231,7 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
     </row>
-    <row r="2" spans="1:6" s="24" customFormat="1" ht="42">
+    <row r="2" spans="1:6" s="24" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -1674,7 +2247,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1694,7 +2267,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>43466</v>
       </c>
@@ -1712,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1">
+    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>43466</v>
       </c>
@@ -1730,7 +2303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1">
+    <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>43466</v>
       </c>
@@ -1748,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1">
+    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>43466</v>
       </c>
@@ -1766,15 +2339,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>43466</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1787,11 +2378,11 @@
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D5</xm:sqref>
+          <xm:sqref>D4:D5 D8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{1BAD95F9-41BA-5842-BA71-6EE162088107}">
           <x14:formula1>
-            <xm:f>'\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
@@ -1806,24 +2397,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="63" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="64" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="64" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="64" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="64" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="64" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="28.83203125" style="63" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="64" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="64" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="64" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="64" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="64" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.95">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>152</v>
       </c>
@@ -1839,7 +2430,7 @@
       <c r="E1" s="59"/>
       <c r="F1" s="59"/>
     </row>
-    <row r="2" spans="1:6" ht="48">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="60"/>
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
@@ -1855,7 +2446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="62" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +2466,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -1893,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -1911,15 +2502,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F6" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1932,11 +2541,11 @@
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D4 D6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{8F00E64D-9BA3-5E44-B5C4-8D0ED00EF488}">
           <x14:formula1>
-            <xm:f>'\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
@@ -1951,23 +2560,23 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1">
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
@@ -1983,7 +2592,7 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
     </row>
-    <row r="2" spans="1:6" s="24" customFormat="1" ht="42">
+    <row r="2" spans="1:6" s="24" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="25" t="s">
@@ -1999,7 +2608,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2019,7 +2628,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>43466</v>
       </c>
@@ -2037,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>43466</v>
       </c>
@@ -2055,7 +2664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1">
+    <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>43466</v>
       </c>
@@ -2073,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1">
+    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>43466</v>
       </c>
@@ -2091,15 +2700,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>43466</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -2112,11 +2739,11 @@
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D5</xm:sqref>
+          <xm:sqref>D4:D5 D8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{53E8C99B-8925-A444-8303-0B51961AB1C2}">
           <x14:formula1>
-            <xm:f>'\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
@@ -2134,22 +2761,22 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
@@ -2168,7 +2795,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" s="24" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" spans="1:9" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="25" t="s">
@@ -2193,7 +2820,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2849,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>43466</v>
       </c>
@@ -2249,7 +2876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>43466</v>
       </c>
@@ -2276,7 +2903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>43466</v>
       </c>
@@ -2303,7 +2930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="7" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>43466</v>
       </c>
@@ -2330,7 +2957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21">
         <v>43466</v>
       </c>
@@ -2357,7 +2984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>43466</v>
       </c>
@@ -2384,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>43466</v>
       </c>
@@ -2411,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>43466</v>
       </c>
@@ -2438,7 +3065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>43466</v>
       </c>
@@ -2465,7 +3092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>43466</v>
       </c>
@@ -2492,7 +3119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>43466</v>
       </c>
@@ -2519,7 +3146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="15" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>43466</v>
       </c>
@@ -2546,17 +3173,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="21"/>
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
+        <v>43466</v>
+      </c>
       <c r="B16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="C16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="D17" s="22"/>
@@ -2566,7 +3210,7 @@
       <c r="H17" s="35"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="18" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="D18" s="22"/>
@@ -2576,7 +3220,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="D19" s="22"/>
@@ -2586,7 +3230,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="20" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="D20" s="22"/>
@@ -2596,7 +3240,7 @@
       <c r="H20" s="35"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="21" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="D21" s="22"/>
@@ -2606,7 +3250,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
     </row>
-    <row r="22" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="22" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="D22" s="22"/>
@@ -2616,7 +3260,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
     </row>
-    <row r="23" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="23" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="D23" s="22"/>
@@ -2626,7 +3270,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
     </row>
-    <row r="24" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="24" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="D24" s="22"/>
@@ -2636,7 +3280,7 @@
       <c r="H24" s="35"/>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="25" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="D25" s="22"/>
@@ -2646,7 +3290,7 @@
       <c r="H25" s="35"/>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="26" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="D26" s="22"/>
@@ -2656,7 +3300,7 @@
       <c r="H26" s="35"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="27" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="D27" s="22"/>
@@ -2666,7 +3310,7 @@
       <c r="H27" s="35"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="28" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
       <c r="B28" s="21"/>
       <c r="D28" s="22"/>
@@ -2676,7 +3320,7 @@
       <c r="H28" s="35"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="29" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="D29" s="22"/>
@@ -2686,7 +3330,7 @@
       <c r="H29" s="35"/>
       <c r="I29" s="22"/>
     </row>
-    <row r="30" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="30" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="D30" s="22"/>
@@ -2696,7 +3340,7 @@
       <c r="H30" s="35"/>
       <c r="I30" s="22"/>
     </row>
-    <row r="31" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="31" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="D31" s="22"/>
@@ -2706,7 +3350,7 @@
       <c r="H31" s="35"/>
       <c r="I31" s="22"/>
     </row>
-    <row r="32" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="32" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="D32" s="22"/>
@@ -2716,7 +3360,7 @@
       <c r="H32" s="35"/>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="33" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="D33" s="22"/>
@@ -2726,7 +3370,7 @@
       <c r="H33" s="35"/>
       <c r="I33" s="22"/>
     </row>
-    <row r="34" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="D34" s="22"/>
@@ -2736,7 +3380,7 @@
       <c r="H34" s="35"/>
       <c r="I34" s="22"/>
     </row>
-    <row r="35" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="35" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="D35" s="22"/>
@@ -2746,7 +3390,7 @@
       <c r="H35" s="35"/>
       <c r="I35" s="22"/>
     </row>
-    <row r="36" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="D36" s="22"/>
@@ -2758,7 +3402,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I36 G4:G36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
@@ -2786,17 +3430,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="53.5" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="25.5" customHeight="1">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -2811,7 +3455,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="31" customFormat="1">
+    <row r="3" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="30" t="s">
         <v>7</v>
       </c>
@@ -2831,7 +3475,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="65">
         <v>43466</v>
       </c>
@@ -2865,21 +3509,21 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>176</v>
       </c>
@@ -2894,7 +3538,7 @@
       </c>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="69.95">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="25" t="s">
@@ -2907,7 +3551,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.95">
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="80" t="s">
         <v>7</v>
       </c>
@@ -2924,7 +3568,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="11" customFormat="1" ht="12.95">
+    <row r="4" spans="1:5" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="23">
         <v>43466</v>
       </c>
@@ -2939,7 +3583,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.95">
+    <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="23">
         <v>43466</v>
       </c>
@@ -2954,7 +3598,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="12.95">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="23">
         <v>43466</v>
       </c>
@@ -2966,6 +3610,36 @@
         <v>183</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="23">
+        <v>43466</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2982,24 +3656,24 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="54" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="54" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="54" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="54" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="54" customWidth="1"/>
     <col min="5" max="5" width="27" style="54" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="54" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="47"/>
+    <col min="6" max="6" width="14.5" style="54" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>184</v>
       </c>
@@ -3015,7 +3689,7 @@
       <c r="E1" s="46"/>
       <c r="F1" s="46"/>
     </row>
-    <row r="2" spans="1:6" ht="69.95">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -3031,7 +3705,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.95" customHeight="1">
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
@@ -3051,7 +3725,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.95" customHeight="1">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="52">
         <v>43466</v>
       </c>
@@ -3069,7 +3743,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.95" customHeight="1">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="52">
         <v>43466</v>
       </c>
@@ -3087,7 +3761,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.95" customHeight="1">
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="52">
         <v>43466</v>
       </c>
@@ -3105,7 +3779,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="12.95" customHeight="1">
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="52">
         <v>43466</v>
       </c>
@@ -3123,7 +3797,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12.95" customHeight="1">
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="52">
         <v>43466</v>
       </c>
@@ -3141,7 +3815,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.95" customHeight="1">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="52">
         <v>43466</v>
       </c>
@@ -3159,7 +3833,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.95" customHeight="1">
+    <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="52">
         <v>43466</v>
       </c>
@@ -3177,7 +3851,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="12.95" customHeight="1">
+    <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="52">
         <v>43466</v>
       </c>
@@ -3195,7 +3869,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.95" customHeight="1">
+    <row r="12" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="52">
         <v>43466</v>
       </c>
@@ -3210,6 +3884,42 @@
         <v>183</v>
       </c>
       <c r="F12" s="66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="52">
+        <v>43466</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="52">
+        <v>43466</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="66" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3228,20 +3938,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>187</v>
       </c>
@@ -3257,7 +3967,7 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
     </row>
-    <row r="2" spans="1:6" s="24" customFormat="1" ht="84">
+    <row r="2" spans="1:6" s="24" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -3273,7 +3983,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="27" customFormat="1" ht="12.95">
+    <row r="3" spans="1:6" s="27" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="80" t="s">
         <v>7</v>
       </c>
@@ -3293,7 +4003,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="65">
         <v>43466</v>
       </c>
@@ -3310,7 +4020,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="65">
         <v>43466</v>
       </c>
@@ -3327,7 +4037,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="65">
         <v>43466</v>
       </c>
@@ -3344,7 +4054,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="65">
         <v>43466</v>
       </c>
@@ -3361,7 +4071,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="65">
         <v>43466</v>
       </c>
@@ -3378,7 +4088,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="65">
         <v>43466</v>
       </c>
@@ -3395,7 +4105,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="65">
         <v>43466</v>
       </c>
@@ -3412,7 +4122,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="65">
         <v>43466</v>
       </c>
@@ -3429,7 +4139,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="65">
         <v>43466</v>
       </c>
@@ -3446,7 +4156,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="65">
         <v>43466</v>
       </c>
@@ -3463,7 +4173,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="65">
         <v>43466</v>
       </c>
@@ -3480,7 +4190,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="65">
         <v>43466</v>
       </c>
@@ -3497,7 +4207,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="65">
         <v>43466</v>
       </c>
@@ -3514,15 +4224,25 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
-      <c r="A17" s="11"/>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="65">
+        <v>43466</v>
+      </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+      <c r="C17" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -3530,7 +4250,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3538,7 +4258,7 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -3546,7 +4266,7 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -3570,19 +4290,19 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>188</v>
       </c>
@@ -3598,7 +4318,7 @@
       <c r="E1" s="22"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="69.95">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
@@ -3614,7 +4334,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="27" customFormat="1" ht="12.95">
+    <row r="3" spans="1:6" s="27" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="80" t="s">
         <v>7</v>
       </c>
@@ -3634,7 +4354,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="65">
         <v>43466</v>
       </c>
@@ -3651,7 +4371,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="65">
         <v>43466</v>
       </c>
@@ -3668,7 +4388,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="65">
         <v>43466</v>
       </c>
@@ -3685,7 +4405,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="65">
         <v>43466</v>
       </c>
@@ -3702,7 +4422,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="65">
         <v>43466</v>
       </c>
@@ -3719,7 +4439,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="65">
         <v>43466</v>
       </c>
@@ -3736,7 +4456,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="65">
         <v>43466</v>
       </c>
@@ -3754,7 +4474,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="65">
         <v>43466</v>
       </c>
@@ -3771,7 +4491,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="65">
         <v>43466</v>
       </c>
@@ -3788,7 +4508,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="65">
         <v>43466</v>
       </c>
@@ -3805,7 +4525,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="65">
         <v>43466</v>
       </c>
@@ -3822,7 +4542,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="65">
         <v>43466</v>
       </c>
@@ -3839,7 +4559,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="65">
         <v>43466</v>
       </c>
@@ -3856,7 +4576,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="17" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="65">
         <v>43466</v>
       </c>
@@ -3873,7 +4593,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="18" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="65">
         <v>43466</v>
       </c>
@@ -3890,7 +4610,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="19" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="65">
         <v>43466</v>
       </c>
@@ -3907,7 +4627,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="20" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="65">
         <v>43466</v>
       </c>
@@ -3924,7 +4644,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="65">
         <v>43466</v>
       </c>
@@ -3941,20 +4661,42 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="65"/>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="65">
+        <v>43466</v>
+      </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="65"/>
-      <c r="D23" s="35"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+      <c r="C22" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="65">
+        <v>43466</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="65"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -3962,92 +4704,92 @@
       <c r="E24" s="11"/>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="25" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="65"/>
       <c r="D25" s="35"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="26" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="65"/>
       <c r="D26" s="35"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="27" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="65"/>
       <c r="D27" s="22"/>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="28" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="65"/>
       <c r="D28" s="22"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="29" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="65"/>
       <c r="D29" s="22"/>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="65"/>
       <c r="D30" s="35"/>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="31" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="65"/>
       <c r="D31" s="35"/>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="32" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="65"/>
       <c r="D32" s="35"/>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="33" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="65"/>
       <c r="D33" s="35"/>
       <c r="F33" s="19"/>
     </row>
-    <row r="34" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="34" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="65"/>
       <c r="D34" s="35"/>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="35" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="65"/>
       <c r="D35" s="35"/>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="36" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="65"/>
       <c r="D36" s="35"/>
       <c r="F36" s="19"/>
     </row>
-    <row r="37" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="37" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="65"/>
       <c r="D37" s="35"/>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="38" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="65"/>
       <c r="D38" s="19"/>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="39" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="65"/>
       <c r="D39" s="35"/>
       <c r="F39" s="19"/>
     </row>
-    <row r="40" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="40" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="65"/>
       <c r="D40" s="35"/>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="41" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="65"/>
       <c r="D41" s="35"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1">
+    <row r="42" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="65"/>
       <c r="D42" s="35"/>
       <c r="F42" s="19"/>
@@ -4068,22 +4810,22 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="72" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="72" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="72" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="72" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.7109375" style="72" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="72" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="72" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="72"/>
+    <col min="1" max="1" width="33.1640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="72" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>189</v>
       </c>
@@ -4100,7 +4842,7 @@
       <c r="F1" s="71"/>
       <c r="G1" s="71"/>
     </row>
-    <row r="2" spans="1:7" ht="69.95">
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="73"/>
       <c r="B2" s="73"/>
       <c r="C2" s="74" t="s">
@@ -4119,7 +4861,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="75" t="s">
         <v>7</v>
       </c>
@@ -4142,21 +4884,21 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="65"/>
       <c r="C4" s="11"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
       <c r="F4" s="53"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="65"/>
       <c r="C5" s="11"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="53"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="65"/>
       <c r="C6" s="11"/>
       <c r="D6" s="35"/>
@@ -4173,23 +4915,23 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4208,7 +4950,7 @@
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
     </row>
-    <row r="2" spans="1:9" s="24" customFormat="1" ht="74.099999999999994" customHeight="1">
+    <row r="2" spans="1:9" s="24" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -4233,7 +4975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -4262,7 +5004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -4285,7 +5027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -4306,15 +5048,41 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="10:10" ht="15" customHeight="1">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C8" s="22"/>
+    </row>
+    <row r="26" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J26" s="78"/>
     </row>
   </sheetData>
   <dataValidations xWindow="279" yWindow="381" count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4328,30 +5096,693 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BEB145-4E89-004E-B749-FD65594B6305}">
+  <dimension ref="A1:H58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" style="86" customWidth="1"/>
+    <col min="2" max="4" width="11.5" style="86"/>
+    <col min="5" max="5" width="38.5" style="86" customWidth="1"/>
+    <col min="6" max="6" width="75.83203125" style="86" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="86"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="83"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="85"/>
+    </row>
+    <row r="2" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+      <c r="A2" s="87" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="89" t="s">
+        <v>205</v>
+      </c>
+      <c r="G3" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="90" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="91">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="91"/>
+      <c r="C4" s="92" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="94" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" s="95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="91">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="92" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="92"/>
+      <c r="E5" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="H5" s="95" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="97"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="95"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="95"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="95"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="95"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="91"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="95"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="91"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="91"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="95"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="91"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="95"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="91"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="95"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="95"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="95"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="91"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="95"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="91"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="95"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="91"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="95"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="91"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="95"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="95"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="95"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="95"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="91"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="95"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="91"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="95"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="91"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="95"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="91"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="92"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="95"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="91"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="95"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="91"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="95"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="95"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="91"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="92"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="95"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="91"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="95"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="91"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="95"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="91"/>
+      <c r="B36" s="91"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="100"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="95"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="91"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="95"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38" s="91"/>
+      <c r="B38" s="91"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="100"/>
+      <c r="F38" s="101"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="95"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="91"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="100"/>
+      <c r="F39" s="101"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="95"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="91"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="95"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41" s="91"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="101"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="95"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42" s="91"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="101"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="95"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A43" s="91"/>
+      <c r="B43" s="91"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="95"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A44" s="91"/>
+      <c r="B44" s="91"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="95"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A45" s="91"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="95"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A46" s="91"/>
+      <c r="B46" s="91"/>
+      <c r="C46" s="98"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="95"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A47" s="91"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="93"/>
+      <c r="F47" s="93"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="95"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48" s="91"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="95"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="91"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="98"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="93"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="98"/>
+      <c r="H49" s="95"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50" s="91"/>
+      <c r="B50" s="91"/>
+      <c r="C50" s="98"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="93"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="95"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A51" s="91"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="98"/>
+      <c r="D51" s="98"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="98"/>
+      <c r="H51" s="95"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A52" s="91"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="98"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="98"/>
+      <c r="H52" s="95"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53" s="91"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="93"/>
+      <c r="F53" s="93"/>
+      <c r="G53" s="98"/>
+      <c r="H53" s="95"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54" s="91"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="98"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="93"/>
+      <c r="F54" s="93"/>
+      <c r="G54" s="98"/>
+      <c r="H54" s="95"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A55" s="91"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="98"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="93"/>
+      <c r="F55" s="93"/>
+      <c r="G55" s="98"/>
+      <c r="H55" s="95"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A56" s="103"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="98"/>
+      <c r="D56" s="98"/>
+      <c r="E56" s="93"/>
+      <c r="F56" s="93"/>
+      <c r="G56" s="98"/>
+      <c r="H56" s="95"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A57" s="103"/>
+      <c r="B57" s="103"/>
+      <c r="C57" s="98"/>
+      <c r="D57" s="98"/>
+      <c r="E57" s="93"/>
+      <c r="F57" s="93"/>
+      <c r="G57" s="98"/>
+      <c r="H57" s="95"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A58" s="104"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="105"/>
+      <c r="D58" s="105"/>
+      <c r="E58" s="106"/>
+      <c r="F58" s="106"/>
+      <c r="G58" s="105"/>
+      <c r="H58" s="107"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="7" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" customWidth="1"/>
+    <col min="12" max="13" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -4374,7 +5805,7 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13" s="24" customFormat="1" ht="51.75" customHeight="1">
+    <row r="2" spans="1:13" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -4407,7 +5838,7 @@
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1">
+    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -4448,7 +5879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -4479,7 +5910,7 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -4508,7 +5939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>43466</v>
       </c>
@@ -4537,7 +5968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="7" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>43466</v>
       </c>
@@ -4566,7 +5997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>43466</v>
       </c>
@@ -4595,7 +6026,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="9" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>43466</v>
       </c>
@@ -4624,7 +6055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="10" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>43466</v>
       </c>
@@ -4653,7 +6084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="11" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>43466</v>
       </c>
@@ -4682,7 +6113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="12" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>43466</v>
       </c>
@@ -4711,7 +6142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="13" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>43466</v>
       </c>
@@ -4740,7 +6171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>43466</v>
       </c>
@@ -4769,7 +6200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="15" spans="1:13" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>43466</v>
       </c>
@@ -4798,12 +6229,41 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15 A16" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B15 B16" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4825,15 +6285,15 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -4848,7 +6308,7 @@
       </c>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -4861,7 +6321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -4878,77 +6338,77 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
       <c r="E6" s="35"/>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
       <c r="E7" s="35"/>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="35"/>
     </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
     </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="10" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="12" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="13" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
     </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:5" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="35"/>
@@ -4981,24 +6441,24 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="11" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="14" width="8.85546875" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -5022,7 +6482,7 @@
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="51.75" customHeight="1">
+    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
@@ -5058,7 +6518,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -5102,7 +6562,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="4" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="6"/>
       <c r="C4" s="35"/>
@@ -5118,7 +6578,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="6"/>
       <c r="C5" s="35"/>
@@ -5134,7 +6594,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="13"/>
       <c r="C6" s="35"/>
@@ -5150,7 +6610,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="7" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10"/>
       <c r="B7" s="13"/>
       <c r="C7" s="35"/>
@@ -5164,7 +6624,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:14" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="13"/>
       <c r="C8" s="35"/>
@@ -5198,24 +6658,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -5232,7 +6692,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:7" ht="60.95" customHeight="1">
+    <row r="2" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -5245,7 +6705,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -5268,7 +6728,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -5287,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -5306,7 +6766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>43466</v>
       </c>
@@ -5325,7 +6785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="7" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>43466</v>
       </c>
@@ -5344,7 +6804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>43466</v>
       </c>
@@ -5363,7 +6823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="9" spans="1:7" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>43466</v>
       </c>
@@ -5382,15 +6842,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G9" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G10" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A10" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5406,34 +6885,34 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16:Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="45.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="45.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="24" customWidth="1"/>
-    <col min="12" max="12" width="31.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.85546875" style="24" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" style="24" customWidth="1"/>
-    <col min="16" max="16" width="23.7109375" customWidth="1"/>
-    <col min="17" max="17" width="31.140625" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="24" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" style="24" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
@@ -5454,7 +6933,7 @@
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
     </row>
-    <row r="2" spans="1:17" ht="84">
+    <row r="2" spans="1:17" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
@@ -5503,7 +6982,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -5556,7 +7035,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -5585,7 +7064,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -5622,7 +7101,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="6" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>43466</v>
       </c>
@@ -5659,7 +7138,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="7" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>43466</v>
       </c>
@@ -5696,7 +7175,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="8" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>43466</v>
       </c>
@@ -5733,7 +7212,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="9" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>43466</v>
       </c>
@@ -5770,7 +7249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="10" spans="1:17" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>43466</v>
       </c>
@@ -5805,7 +7284,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>43466</v>
       </c>
@@ -5842,7 +7321,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="12" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>43466</v>
       </c>
@@ -5879,7 +7358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="13" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>43466</v>
       </c>
@@ -5916,7 +7395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="14" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>43466</v>
       </c>
@@ -5953,7 +7432,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1">
+    <row r="15" spans="1:17" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>43466</v>
       </c>
@@ -5990,15 +7469,44 @@
         <v>51</v>
       </c>
     </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G15" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G16" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A15" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A16" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
   </dataValidations>
@@ -6017,28 +7525,28 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="7" width="20.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" style="11" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="20.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" customWidth="1"/>
+    <col min="14" max="14" width="28.6640625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
@@ -6062,7 +7570,7 @@
       <c r="M1" s="11"/>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" s="40" customFormat="1" ht="54.75" customHeight="1">
+    <row r="2" spans="1:15" s="40" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36" t="s">
@@ -6105,7 +7613,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -6152,7 +7660,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1">
+    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -6190,7 +7698,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -6227,7 +7735,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="6" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>43466</v>
       </c>
@@ -6264,7 +7772,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="7" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>43466</v>
       </c>
@@ -6301,7 +7809,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>43466</v>
       </c>
@@ -6338,7 +7846,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="9" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>43466</v>
       </c>
@@ -6375,7 +7883,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="10" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10">
         <v>43466</v>
       </c>
@@ -6412,7 +7920,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="11" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10">
         <v>43466</v>
       </c>
@@ -6449,7 +7957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="12" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>43466</v>
       </c>
@@ -6486,7 +7994,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="13" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>43466</v>
       </c>
@@ -6523,7 +8031,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>43466</v>
       </c>
@@ -6560,7 +8068,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="15" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>43466</v>
       </c>
@@ -6597,7 +8105,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="16" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>43466</v>
       </c>
@@ -6634,7 +8142,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>43466</v>
       </c>
@@ -6671,7 +8179,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="18" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10">
         <v>43466</v>
       </c>
@@ -6708,7 +8216,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10">
         <v>43466</v>
       </c>
@@ -6745,7 +8253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="20" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>43466</v>
       </c>
@@ -6782,7 +8290,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="21" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>43466</v>
       </c>
@@ -6819,7 +8327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="22" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
         <v>43466</v>
       </c>
@@ -6856,7 +8364,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="23" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>43466</v>
       </c>
@@ -6893,7 +8401,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="24" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>43466</v>
       </c>
@@ -6930,7 +8438,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="25" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>43466</v>
       </c>
@@ -6967,7 +8475,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="26" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>43466</v>
       </c>
@@ -7004,7 +8512,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="27" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>43466</v>
       </c>
@@ -7041,7 +8549,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="28" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
         <v>43466</v>
       </c>
@@ -7078,7 +8586,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10">
         <v>43466</v>
       </c>
@@ -7115,7 +8623,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="30" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10">
         <v>43466</v>
       </c>
@@ -7152,7 +8660,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="31" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
         <v>43466</v>
       </c>
@@ -7189,7 +8697,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="32" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
         <v>43466</v>
       </c>
@@ -7226,7 +8734,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="33" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10">
         <v>43466</v>
       </c>
@@ -7263,7 +8771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="34" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10">
         <v>43466</v>
       </c>
@@ -7300,7 +8808,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="35" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
         <v>43466</v>
       </c>
@@ -7337,7 +8845,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="36" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
         <v>43466</v>
       </c>
@@ -7374,7 +8882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="37" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10">
         <v>43466</v>
       </c>
@@ -7411,7 +8919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="38" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="10">
         <v>43466</v>
       </c>
@@ -7448,7 +8956,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="39" spans="1:15" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10">
         <v>43466</v>
       </c>
@@ -7506,23 +9014,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -7538,7 +9046,7 @@
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
     </row>
-    <row r="2" spans="1:6" s="24" customFormat="1" ht="42">
+    <row r="2" spans="1:6" s="24" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25" t="s">
@@ -7554,7 +9062,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -7574,7 +9082,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>43466</v>
       </c>
@@ -7592,7 +9100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1">
+    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>43466</v>
       </c>
@@ -7610,15 +9118,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>43466</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F5" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F6" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A5" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7631,11 +9157,11 @@
           <x14:formula1>
             <xm:f>CaseField!$D$4:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D4 D6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{3922A2E3-B39F-854D-BF73-EE32348B2F8C}">
           <x14:formula1>
-            <xm:f>'\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
RDM-13009 - remove ROLE_TO_ACCESS_PROFILE_CASE_TYPE from caseworker-befta_jurisdiction_1 authorisation
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semenu/projects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56307C8C-DDC2-FF48-81D2-76F3B61DA6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31AB5D4-75B7-8344-86A8-1A34E9E06198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" tabRatio="823" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1460" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="213">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -704,12 +704,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>Role2</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>ROLE_TO_ACCESS_PROFILE_CASE_TYPE</t>
@@ -1712,13 +1706,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1728,6 +1715,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1801,7 +1795,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB777435-0AD8-EA4C-A4EE-C9BE1C5AD595}" name="Table2214" displayName="Table2214" ref="A3:H58" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB777435-0AD8-EA4C-A4EE-C9BE1C5AD595}" name="Table2214" displayName="Table2214" ref="A3:H57" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9572B57F-38EA-A146-806B-BFD81A8F93B0}" name="LiveFrom" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{6B9FC0EC-B825-254E-B887-2D066A95169C}" name="LiveTo" dataDxfId="6"/>
@@ -2345,7 +2339,7 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>47</v>
@@ -2382,7 +2376,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{1BAD95F9-41BA-5842-BA71-6EE162088107}">
           <x14:formula1>
-            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
@@ -2508,7 +2502,7 @@
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>47</v>
@@ -2545,7 +2539,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{8F00E64D-9BA3-5E44-B5C4-8D0ED00EF488}">
           <x14:formula1>
-            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
@@ -2706,7 +2700,7 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>47</v>
@@ -2743,7 +2737,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{53E8C99B-8925-A444-8303-0B51961AB1C2}">
           <x14:formula1>
-            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D6:D7</xm:sqref>
         </x14:dataValidation>
@@ -3179,7 +3173,7 @@
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>165</v>
@@ -3509,17 +3503,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3619,27 +3613,12 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>181</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="23">
-        <v>43466</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="11" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3656,10 +3635,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3893,7 +3872,7 @@
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>83</v>
@@ -3902,24 +3881,6 @@
         <v>181</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="52">
-        <v>43466</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="F14" s="66" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3939,7 +3900,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4230,13 +4191,13 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="53" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>182</v>
@@ -4287,10 +4248,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4667,7 +4628,7 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>47</v>
@@ -4679,29 +4640,17 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="65">
-        <v>43466</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="65"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="65"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="11"/>
       <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4711,7 +4660,7 @@
     </row>
     <row r="26" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="65"/>
-      <c r="D26" s="35"/>
+      <c r="D26" s="22"/>
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4726,7 +4675,7 @@
     </row>
     <row r="29" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="65"/>
-      <c r="D29" s="22"/>
+      <c r="D29" s="35"/>
       <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4766,12 +4715,12 @@
     </row>
     <row r="37" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="65"/>
-      <c r="D37" s="35"/>
+      <c r="D37" s="19"/>
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="65"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="35"/>
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4788,11 +4737,6 @@
       <c r="A41" s="65"/>
       <c r="D41" s="35"/>
       <c r="F41" s="19"/>
-    </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="65"/>
-      <c r="D42" s="35"/>
-      <c r="F42" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4809,7 +4753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -5054,13 +4998,13 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>214</v>
-      </c>
       <c r="E6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>12</v>
@@ -5098,10 +5042,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BEB145-4E89-004E-B749-FD65594B6305}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5187,7 +5131,7 @@
       </c>
       <c r="D4" s="92"/>
       <c r="E4" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>181</v>
@@ -5200,26 +5144,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="91">
-        <v>42736</v>
-      </c>
+      <c r="A5" s="91"/>
       <c r="B5" s="91"/>
-      <c r="C5" s="92" t="s">
-        <v>210</v>
-      </c>
+      <c r="C5" s="92"/>
       <c r="D5" s="92"/>
-      <c r="E5" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" s="93" t="s">
-        <v>211</v>
-      </c>
-      <c r="H5" s="95" t="s">
-        <v>211</v>
-      </c>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="97"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="91"/>
@@ -5228,8 +5160,8 @@
       <c r="D6" s="92"/>
       <c r="E6" s="93"/>
       <c r="F6" s="94"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="95"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="91"/>
@@ -5238,7 +5170,7 @@
       <c r="D7" s="92"/>
       <c r="E7" s="93"/>
       <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
+      <c r="G7" s="93"/>
       <c r="H7" s="95"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -5258,7 +5190,7 @@
       <c r="D9" s="92"/>
       <c r="E9" s="93"/>
       <c r="F9" s="94"/>
-      <c r="G9" s="93"/>
+      <c r="G9" s="94"/>
       <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -5267,7 +5199,7 @@
       <c r="C10" s="92"/>
       <c r="D10" s="92"/>
       <c r="E10" s="93"/>
-      <c r="F10" s="94"/>
+      <c r="F10" s="98"/>
       <c r="G10" s="94"/>
       <c r="H10" s="95"/>
     </row>
@@ -5277,7 +5209,7 @@
       <c r="C11" s="92"/>
       <c r="D11" s="92"/>
       <c r="E11" s="93"/>
-      <c r="F11" s="98"/>
+      <c r="F11" s="94"/>
       <c r="G11" s="94"/>
       <c r="H11" s="95"/>
     </row>
@@ -5286,7 +5218,7 @@
       <c r="B12" s="91"/>
       <c r="C12" s="92"/>
       <c r="D12" s="92"/>
-      <c r="E12" s="93"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="94"/>
       <c r="G12" s="94"/>
       <c r="H12" s="95"/>
@@ -5297,7 +5229,7 @@
       <c r="C13" s="92"/>
       <c r="D13" s="92"/>
       <c r="E13" s="96"/>
-      <c r="F13" s="94"/>
+      <c r="F13" s="96"/>
       <c r="G13" s="94"/>
       <c r="H13" s="95"/>
     </row>
@@ -5307,7 +5239,7 @@
       <c r="C14" s="92"/>
       <c r="D14" s="92"/>
       <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="94"/>
       <c r="H14" s="95"/>
     </row>
@@ -5327,7 +5259,7 @@
       <c r="C16" s="92"/>
       <c r="D16" s="92"/>
       <c r="E16" s="96"/>
-      <c r="F16" s="94"/>
+      <c r="F16" s="93"/>
       <c r="G16" s="94"/>
       <c r="H16" s="95"/>
     </row>
@@ -5337,7 +5269,7 @@
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
       <c r="E17" s="96"/>
-      <c r="F17" s="93"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="94"/>
       <c r="H17" s="95"/>
     </row>
@@ -5366,8 +5298,8 @@
       <c r="B20" s="91"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="99"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
       <c r="G20" s="94"/>
       <c r="H20" s="95"/>
     </row>
@@ -5406,7 +5338,7 @@
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="93"/>
+      <c r="E24" s="92"/>
       <c r="F24" s="93"/>
       <c r="G24" s="94"/>
       <c r="H24" s="95"/>
@@ -5436,7 +5368,7 @@
       <c r="B27" s="91"/>
       <c r="C27" s="92"/>
       <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="93"/>
       <c r="G27" s="94"/>
       <c r="H27" s="95"/>
@@ -5446,9 +5378,9 @@
       <c r="B28" s="91"/>
       <c r="C28" s="92"/>
       <c r="D28" s="92"/>
-      <c r="E28" s="96"/>
+      <c r="E28" s="93"/>
       <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
+      <c r="G28" s="92"/>
       <c r="H28" s="95"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
@@ -5486,9 +5418,9 @@
       <c r="B32" s="91"/>
       <c r="C32" s="92"/>
       <c r="D32" s="92"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="92"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="94"/>
       <c r="H32" s="95"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
@@ -5504,10 +5436,10 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="91"/>
       <c r="B34" s="91"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="96"/>
-      <c r="F34" s="99"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="101"/>
       <c r="G34" s="94"/>
       <c r="H34" s="95"/>
     </row>
@@ -5584,21 +5516,21 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="91"/>
       <c r="B42" s="91"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="100"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="94"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="102"/>
       <c r="H42" s="95"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="91"/>
       <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
+      <c r="C43" s="98"/>
+      <c r="D43" s="98"/>
       <c r="E43" s="93"/>
       <c r="F43" s="93"/>
-      <c r="G43" s="102"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="95"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
@@ -5712,8 +5644,8 @@
       <c r="H54" s="95"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A55" s="91"/>
-      <c r="B55" s="91"/>
+      <c r="A55" s="103"/>
+      <c r="B55" s="103"/>
       <c r="C55" s="98"/>
       <c r="D55" s="98"/>
       <c r="E55" s="93"/>
@@ -5732,24 +5664,14 @@
       <c r="H56" s="95"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A57" s="103"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="98"/>
-      <c r="D57" s="98"/>
-      <c r="E57" s="93"/>
-      <c r="F57" s="93"/>
-      <c r="G57" s="98"/>
-      <c r="H57" s="95"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A58" s="104"/>
-      <c r="B58" s="104"/>
-      <c r="C58" s="105"/>
-      <c r="D58" s="105"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="106"/>
-      <c r="G58" s="105"/>
-      <c r="H58" s="107"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="104"/>
+      <c r="C57" s="105"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="106"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="107"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6235,7 +6157,7 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>47</v>
@@ -6848,7 +6770,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>83</v>
@@ -6887,8 +6809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16:Q16"/>
+    <sheetView topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7475,7 +7397,7 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>105</v>
@@ -9124,7 +9046,7 @@
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>47</v>
@@ -9161,7 +9083,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{3922A2E3-B39F-854D-BF73-EE32348B2F8C}">
           <x14:formula1>
-            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/\Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
+            <xm:f>'/Users/semenu/Library/Containers/com.microsoft.Excel/Data/Documents/Users\sivakanukollu\github\MOJ\ccd-data-store-api\src\aat\resources\[CCD_BEFTA_JURISDICTION4.xlsx]CaseField'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Rename UserRole to AccessProfile
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31AB5D4-75B7-8344-86A8-1A34E9E06198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF670C7-B190-8644-B385-DEF14465540C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1460" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2020" windowWidth="33600" windowHeight="19420" tabRatio="823" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -37,19 +37,10 @@
   <externalReferences>
     <externalReference r:id="rId21"/>
   </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -608,9 +599,6 @@
     <t>Case Events can have Create,Read,Update and Delete. MaxLength: 5</t>
   </si>
   <si>
-    <t>UserRole</t>
-  </si>
-  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -713,6 +701,9 @@
   </si>
   <si>
     <t>RTAP_CASE_TYPE</t>
+  </si>
+  <si>
+    <t>AccessProfile</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2330,7 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>47</v>
@@ -2502,7 +2493,7 @@
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>47</v>
@@ -2700,7 +2691,7 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>47</v>
@@ -3173,7 +3164,7 @@
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>165</v>
@@ -3506,7 +3497,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3556,10 +3547,10 @@
         <v>38</v>
       </c>
       <c r="D3" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="80" t="s">
         <v>179</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3571,10 +3562,10 @@
         <v>24</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -3586,10 +3577,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3601,10 +3592,10 @@
         <v>28</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3613,13 +3604,13 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D7" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3638,7 +3629,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3654,7 +3645,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="43" t="s">
         <v>1</v>
@@ -3678,7 +3669,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>178</v>
@@ -3695,13 +3686,13 @@
         <v>38</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E3" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="50" t="s">
         <v>179</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3716,10 +3707,10 @@
         <v>83</v>
       </c>
       <c r="E4" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="66" t="s">
         <v>181</v>
-      </c>
-      <c r="F4" s="66" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3734,10 +3725,10 @@
         <v>85</v>
       </c>
       <c r="E5" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="66" t="s">
         <v>181</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3752,10 +3743,10 @@
         <v>87</v>
       </c>
       <c r="E6" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="66" t="s">
         <v>181</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3770,10 +3761,10 @@
         <v>83</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F7" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3788,10 +3779,10 @@
         <v>85</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3806,10 +3797,10 @@
         <v>87</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3824,10 +3815,10 @@
         <v>83</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3842,10 +3833,10 @@
         <v>85</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -3860,10 +3851,10 @@
         <v>87</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -3872,16 +3863,16 @@
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>83</v>
       </c>
       <c r="E13" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="66" t="s">
         <v>181</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3900,7 +3891,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3914,7 +3905,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -3938,7 +3929,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="25" t="s">
         <v>178</v>
@@ -3958,10 +3949,10 @@
         <v>129</v>
       </c>
       <c r="E3" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="80" t="s">
         <v>179</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3975,10 +3966,10 @@
         <v>114</v>
       </c>
       <c r="E4" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -3992,10 +3983,10 @@
         <v>105</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4009,10 +4000,10 @@
         <v>108</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4026,10 +4017,10 @@
         <v>110</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4043,10 +4034,10 @@
         <v>112</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4060,10 +4051,10 @@
         <v>114</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4077,10 +4068,10 @@
         <v>117</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4094,10 +4085,10 @@
         <v>105</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4111,10 +4102,10 @@
         <v>108</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4128,10 +4119,10 @@
         <v>110</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4145,10 +4136,10 @@
         <v>112</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4162,10 +4153,10 @@
         <v>114</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4179,10 +4170,10 @@
         <v>117</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4191,16 +4182,16 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4250,8 +4241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4265,7 +4256,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -4309,10 +4300,10 @@
         <v>130</v>
       </c>
       <c r="E3" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="80" t="s">
         <v>179</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4326,10 +4317,10 @@
         <v>47</v>
       </c>
       <c r="E4" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4343,10 +4334,10 @@
         <v>52</v>
       </c>
       <c r="E5" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4360,10 +4351,10 @@
         <v>56</v>
       </c>
       <c r="E6" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4377,10 +4368,10 @@
         <v>60</v>
       </c>
       <c r="E7" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4394,10 +4385,10 @@
         <v>64</v>
       </c>
       <c r="E8" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4411,10 +4402,10 @@
         <v>68</v>
       </c>
       <c r="E9" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4429,10 +4420,10 @@
         <v>47</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4446,10 +4437,10 @@
         <v>52</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4463,10 +4454,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4480,10 +4471,10 @@
         <v>60</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4497,10 +4488,10 @@
         <v>64</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4514,10 +4505,10 @@
         <v>68</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4531,10 +4522,10 @@
         <v>47</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4548,10 +4539,10 @@
         <v>52</v>
       </c>
       <c r="E17" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4565,10 +4556,10 @@
         <v>56</v>
       </c>
       <c r="E18" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4582,10 +4573,10 @@
         <v>60</v>
       </c>
       <c r="E19" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4599,10 +4590,10 @@
         <v>64</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4616,10 +4607,10 @@
         <v>68</v>
       </c>
       <c r="E21" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4628,16 +4619,16 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4753,8 +4744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4771,7 +4762,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>1</v>
@@ -4790,19 +4781,19 @@
       <c r="A2" s="73"/>
       <c r="B2" s="73"/>
       <c r="C2" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="E2" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="F2" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="G2" s="74" t="s">
         <v>193</v>
-      </c>
-      <c r="G2" s="74" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -4822,10 +4813,10 @@
         <v>74</v>
       </c>
       <c r="F3" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="77" t="s">
         <v>179</v>
-      </c>
-      <c r="G3" s="77" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -4998,13 +4989,13 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" t="s">
         <v>210</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="E6" t="s">
-        <v>211</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>12</v>
@@ -5059,7 +5050,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="82"/>
@@ -5073,26 +5064,26 @@
     </row>
     <row r="2" spans="1:8" ht="56" x14ac:dyDescent="0.15">
       <c r="A2" s="87" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="87" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="C2" s="87" t="s">
         <v>197</v>
-      </c>
-      <c r="C2" s="87" t="s">
-        <v>198</v>
       </c>
       <c r="D2" s="87"/>
       <c r="E2" s="87" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="G2" s="87" t="s">
         <v>200</v>
       </c>
-      <c r="G2" s="87" t="s">
+      <c r="H2" s="88" t="s">
         <v>201</v>
-      </c>
-      <c r="H2" s="88" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -5103,22 +5094,22 @@
         <v>8</v>
       </c>
       <c r="C3" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="89" t="s">
         <v>203</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>204</v>
       </c>
       <c r="E3" s="89" t="s">
         <v>38</v>
       </c>
       <c r="F3" s="89" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="G3" s="89" t="s">
-        <v>206</v>
-      </c>
       <c r="H3" s="90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
@@ -5127,20 +5118,20 @@
       </c>
       <c r="B4" s="91"/>
       <c r="C4" s="92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="92"/>
       <c r="E4" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4" s="95" t="s">
         <v>208</v>
-      </c>
-      <c r="H4" s="95" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -6157,7 +6148,7 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>47</v>
@@ -6770,7 +6761,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>83</v>
@@ -7397,7 +7388,7 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>105</v>
@@ -9046,7 +9037,7 @@
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
bumping version + Missing bits + spelling typo
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F452D6-9190-6343-A5AA-7DC5286FA229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4DAA1-60F0-5844-BE05-AE5EC23C6812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" firstSheet="17" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -809,19 +809,7 @@
     <t>OGD_DWP_PROFILE</t>
   </si>
   <si>
-    <t>BEFTA bulk Solicitor 2  Respondant for Org description2</t>
-  </si>
-  <si>
-    <t>BEFTA bulk Solicitor 2 Respondant for Org hint2</t>
-  </si>
-  <si>
     <t>SOLICITOR_PROFILE</t>
-  </si>
-  <si>
-    <t>BEFTA Solicitor Profile  Respondant for Org description</t>
-  </si>
-  <si>
-    <t>BEFTA Solicitor Profile Respondant for Org hint</t>
   </si>
   <si>
     <t>AccessTypeRole</t>
@@ -872,6 +860,18 @@
   </si>
   <si>
     <t>GroupRole2</t>
+  </si>
+  <si>
+    <t>BEFTA bulk Solicitor 2  Respondent for Org description2</t>
+  </si>
+  <si>
+    <t>BEFTA Solicitor Profile  Respondent for Org description</t>
+  </si>
+  <si>
+    <t>BEFTA bulk Solicitor 2 Respondent for Org hint2</t>
+  </si>
+  <si>
+    <t>BEFTA Solicitor Profile Respondent for Org hint</t>
   </si>
 </sst>
 </file>
@@ -1752,13 +1752,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1794,6 +1787,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2080,13 +2080,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2122,6 +2115,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2356,7 +2356,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65A2D01F-663C-9C40-B22C-87DBBFDB8C8B}" name="Table230" displayName="Table230" ref="A3:K127" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" headerRowBorderDxfId="27" tableBorderDxfId="28" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{65A2D01F-663C-9C40-B22C-87DBBFDB8C8B}" name="Table230" displayName="Table230" ref="A3:K127" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A3:K127" xr:uid="{65A2D01F-663C-9C40-B22C-87DBBFDB8C8B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4240DAB0-6802-604C-AFD6-1DA3C13ABECC}" name="LiveFrom" dataDxfId="25"/>
@@ -2376,7 +2376,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{57BDFF47-3DBE-4742-8547-AFE89CA592C2}" name="Table23031" displayName="Table23031" ref="A3:J127" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{57BDFF47-3DBE-4742-8547-AFE89CA592C2}" name="Table23031" displayName="Table23031" ref="A3:J127" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A3:J127" xr:uid="{57BDFF47-3DBE-4742-8547-AFE89CA592C2}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{E806FDD9-0904-DD4C-A529-5667C9E1E0B2}" name="LiveFrom" dataDxfId="9"/>
@@ -5575,7 +5575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -5660,7 +5660,7 @@
       </c>
       <c r="B4" s="108"/>
       <c r="C4" s="103" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D4" s="103"/>
       <c r="E4" s="111" t="s">
@@ -5682,7 +5682,7 @@
       </c>
       <c r="B5" s="108"/>
       <c r="C5" s="103" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D5" s="103"/>
       <c r="E5" s="111" t="s">
@@ -6207,8 +6207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5C47FB-35CD-9F4C-85BA-572C3A9AC421}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6329,10 +6329,10 @@
         <v>123</v>
       </c>
       <c r="I4" s="101" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="K4" s="102">
         <v>1</v>
@@ -6350,7 +6350,7 @@
         <v>243</v>
       </c>
       <c r="E5" s="101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F5" s="101" t="s">
         <v>123</v>
@@ -6362,10 +6362,10 @@
         <v>123</v>
       </c>
       <c r="I5" s="101" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="J5" s="102" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="K5" s="102">
         <v>2</v>
@@ -7815,7 +7815,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="91"/>
@@ -7838,19 +7838,19 @@
         <v>231</v>
       </c>
       <c r="F2" s="97" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="97" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="95" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="96" t="s">
         <v>251</v>
-      </c>
-      <c r="G2" s="97" t="s">
-        <v>252</v>
-      </c>
-      <c r="H2" s="95" t="s">
-        <v>253</v>
-      </c>
-      <c r="I2" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="J2" s="96" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -7870,19 +7870,19 @@
         <v>239</v>
       </c>
       <c r="F3" s="110" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" s="98" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="98" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="98" t="s">
         <v>256</v>
-      </c>
-      <c r="G3" s="98" t="s">
-        <v>257</v>
-      </c>
-      <c r="H3" s="98" t="s">
-        <v>258</v>
-      </c>
-      <c r="I3" s="98" t="s">
-        <v>259</v>
-      </c>
-      <c r="J3" s="98" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -7900,19 +7900,19 @@
         <v>244</v>
       </c>
       <c r="F4" s="102" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G4" s="101" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H4" s="102" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I4" s="102" t="s">
         <v>123</v>
       </c>
       <c r="J4" s="102" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -7930,11 +7930,11 @@
         <v>244</v>
       </c>
       <c r="F5" s="102" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G5" s="101"/>
       <c r="H5" s="102" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I5" s="102" t="s">
         <v>123</v>
@@ -7953,22 +7953,22 @@
         <v>243</v>
       </c>
       <c r="E6" s="101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F6" s="102" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G6" s="101" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H6" s="102" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I6" s="102" t="s">
         <v>123</v>
       </c>
       <c r="J6" s="102" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -7983,14 +7983,14 @@
         <v>243</v>
       </c>
       <c r="E7" s="101" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G7" s="101"/>
       <c r="H7" s="102" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I7" s="102" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
added befta.caseworker.1@gmail.com for CaseAccessGroups_Casetype
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4DAA1-60F0-5844-BE05-AE5EC23C6812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37831988-4C9B-654F-8AB0-260AD915C004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33720" yWindow="500" windowWidth="33720" windowHeight="21100" tabRatio="500" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="265">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3888,10 +3888,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A4:XFD4 A5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3956,9 +3956,27 @@
         <v>95</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{84B4E984-A416-A64A-918C-D95C14E8BE8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5385,7 +5403,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" activeCellId="1" sqref="A4:XFD4 A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6207,7 +6225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5C47FB-35CD-9F4C-85BA-572C3A9AC421}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rolledback change as this is not the issue. i.e. befta.caseworker.1@gmail.com for CaseAccessGroups_Casetype
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37831988-4C9B-654F-8AB0-260AD915C004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A219AB3-28B3-3F42-92C1-AE12715260CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33720" yWindow="500" windowWidth="33720" windowHeight="21100" tabRatio="500" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="980" windowWidth="17200" windowHeight="21580" tabRatio="500" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="265">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3891,7 +3891,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3957,26 +3957,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="30">
-        <v>43466</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="A5" s="30"/>
+      <c r="C5" s="42"/>
+      <c r="F5" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{84B4E984-A416-A64A-918C-D95C14E8BE8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Changes to Access for accessing CaseAccessGroups_Casetype in FT's for ccd-store-api
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A219AB3-28B3-3F42-92C1-AE12715260CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2FEEC1-BD54-704D-A8C5-A7AC095E8C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="980" windowWidth="17200" windowHeight="21580" tabRatio="500" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="500" windowWidth="30220" windowHeight="19880" tabRatio="500" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
   <externalReferences>
     <externalReference r:id="rId23"/>
   </externalReferences>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="266">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -872,6 +872,9 @@
   </si>
   <si>
     <t>BEFTA Solicitor Profile Respondent for Org hint</t>
+  </si>
+  <si>
+    <t>idam:caseworker-befta_jurisdiction_1</t>
   </si>
 </sst>
 </file>
@@ -3890,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -5580,8 +5583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5703,15 +5706,26 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="81"/>
+    <row r="6" spans="1:8" s="102" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="100">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="100"/>
+      <c r="C6" s="102" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="111" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="102" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="101" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="77"/>

</xml_diff>

<commit_message>
Changes for testing AC02B: Error response for unauthorised access by Internal Parties
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2FEEC1-BD54-704D-A8C5-A7AC095E8C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D5C55-66FB-BC43-B3F1-4DA54F7E0E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="500" windowWidth="30220" windowHeight="19880" tabRatio="500" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="33720" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="269">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -875,6 +875,15 @@
   </si>
   <si>
     <t>idam:caseworker-befta_jurisdiction_1</t>
+  </si>
+  <si>
+    <t>BEFTA_CASETYPE_NO_READ</t>
+  </si>
+  <si>
+    <t>BEFTA Case Type No Read</t>
+  </si>
+  <si>
+    <t>Create a case of type BEFTA_CASETYPE_NO_READ</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1315,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1515,6 +1524,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2668,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" activeCellId="1" sqref="A4:XFD4 A10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2775,8 +2785,8 @@
         <v>43466</v>
       </c>
       <c r="B6" s="29"/>
-      <c r="C6" t="s">
-        <v>28</v>
+      <c r="C6" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>52</v>
@@ -2793,8 +2803,8 @@
         <v>43466</v>
       </c>
       <c r="B7" s="29"/>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="C7" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>69</v>
@@ -2806,13 +2816,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
         <v>43466</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>52</v>
@@ -2824,34 +2834,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <v>43466</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>43466</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>45266</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E11" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F11" s="29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F11" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2863,12 +2909,12 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$9</xm:f>
+            <xm:f>CaseField!$D$10:$D$15</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D4:D5 D8</xm:sqref>
+          <xm:sqref>D4:D7 D10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
@@ -2877,7 +2923,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D6:D7</xm:sqref>
+          <xm:sqref>D8:D9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2887,10 +2933,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" activeCellId="1" sqref="A4:XFD4 C7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2978,8 +3024,8 @@
         <v>43466</v>
       </c>
       <c r="B5" s="28"/>
-      <c r="C5" t="s">
-        <v>28</v>
+      <c r="C5" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -2991,13 +3037,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43466</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
@@ -3009,16 +3055,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>45266</v>
-      </c>
-      <c r="B7"/>
+        <v>43466</v>
+      </c>
+      <c r="B7" s="28"/>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>167</v>
@@ -3027,18 +3073,40 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>45266</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{5CDF4AE9-AA1A-C448-9DC6-810CCBA3C49A}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{1BB6D401-03B3-944D-A92C-CF1B8F31F045}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0A00-000002000000}">
-      <formula1>IF((DATEDIF(A7,B7,"d")&gt;0),B7)</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{D38E398C-303C-4A4B-826A-8DC53C033CE3}">
+      <formula1>IF((DATEDIF(A8,B8,"d")&gt;0),B8)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B6:B7" xr:uid="{363C8EA3-7842-DE45-B9F3-9DD5A9224071}">
+      <formula1>IF((DATEDIF(A9,B9,"d")&gt;0),B9)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3047,23 +3115,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{75921CDF-8B71-FC48-B818-7C7FB90556C3}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$9</xm:f>
+            <xm:f>CaseField!$D$10:$D$15</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D4 D6</xm:sqref>
+          <xm:sqref>D7 D4:D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{3835A067-4B97-924A-97FD-05520DCB91E3}">
           <x14:formula1>
             <xm:f>'/users/semenu/library/containers/com.microsoft.excel/data/documents/users\sivakanukollu\github\moj\ccd-data-store-api\src\aat\resources\[ccd_befta_jurisdiction4.xlsx]casefield'!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D5</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3073,10 +3141,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" activeCellId="1" sqref="A4:XFD4 D28"/>
+    <sheetView topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3180,8 +3248,8 @@
         <v>43466</v>
       </c>
       <c r="B6" s="29"/>
-      <c r="C6" t="s">
-        <v>28</v>
+      <c r="C6" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>52</v>
@@ -3198,8 +3266,8 @@
         <v>43466</v>
       </c>
       <c r="B7" s="29"/>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="C7" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>69</v>
@@ -3211,13 +3279,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
         <v>43466</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>52</v>
@@ -3229,34 +3297,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <v>43466</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>43466</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>45266</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E11" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F11" s="29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A11" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F11" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3268,12 +3372,12 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$9</xm:f>
+            <xm:f>CaseField!$D$10:$D$15</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D4:D5 D8</xm:sqref>
+          <xm:sqref>D10 D4:D7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
@@ -3282,7 +3386,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D6:D7</xm:sqref>
+          <xm:sqref>D8:D9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3292,10 +3396,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E34" activeCellId="1" sqref="A4:XFD4 E34"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3546,8 +3650,8 @@
         <v>43466</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D10" t="s">
         <v>185</v>
@@ -3573,8 +3677,8 @@
         <v>43466</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D11" t="s">
         <v>185</v>
@@ -3600,8 +3704,8 @@
         <v>43466</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="C12" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D12" t="s">
         <v>185</v>
@@ -3627,8 +3731,8 @@
         <v>43466</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" t="s">
-        <v>28</v>
+      <c r="C13" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D13" t="s">
         <v>185</v>
@@ -3654,8 +3758,8 @@
         <v>43466</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D14" t="s">
         <v>185</v>
@@ -3681,8 +3785,8 @@
         <v>43466</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D15" t="s">
         <v>185</v>
@@ -3709,7 +3813,7 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>185</v>
@@ -3730,101 +3834,221 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
-        <v>45266</v>
+        <v>43466</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>185</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>187</v>
       </c>
       <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17">
         <v>2</v>
       </c>
-      <c r="H17" t="s">
-        <v>77</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <v>45266</v>
+        <v>43466</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
         <v>185</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>82</v>
+        <v>186</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>187</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8">
+        <v>45266</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8">
+        <v>45266</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
         <v>81</v>
       </c>
-      <c r="I18">
+      <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="29"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="29"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="29"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="29"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="29"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="29"/>
-      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
@@ -3868,18 +4092,59 @@
       <c r="F30" s="29"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="29"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="29"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="29"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="29"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="29"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="29"/>
+      <c r="H36" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A30" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G30 I4:I30" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I36 G4:G36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B30" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3977,8 +4242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" activeCellId="1" sqref="A4:XFD4 C19"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4069,8 +4334,8 @@
         <v>43466</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" t="s">
-        <v>28</v>
+      <c r="C6" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D6" t="s">
         <v>204</v>
@@ -4079,46 +4344,60 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="43">
         <v>43466</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>202</v>
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>204</v>
       </c>
       <c r="E7" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8">
+      <c r="A8" s="43">
+        <v>43466</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8">
         <v>45266</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>204</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A8" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A9" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B8" xr:uid="{00000000-0002-0000-0E00-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B9" xr:uid="{00000000-0002-0000-0E00-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4130,10 +4409,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" activeCellId="1" sqref="A4:XFD4 D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4312,14 +4591,14 @@
         <v>43466</v>
       </c>
       <c r="B10" s="49"/>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>203</v>
@@ -4330,14 +4609,14 @@
         <v>43466</v>
       </c>
       <c r="B11" s="49"/>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>97</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
         <v>203</v>
@@ -4348,80 +4627,188 @@
         <v>43466</v>
       </c>
       <c r="B12" s="49"/>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="C12" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="54">
         <v>43466</v>
       </c>
       <c r="B13" s="49"/>
-      <c r="C13" t="s">
-        <v>31</v>
+      <c r="C13" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="54">
+        <v>43466</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8">
         <v>45266</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E20" t="s">
         <v>204</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8">
         <v>45266</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E21" t="s">
         <v>204</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>201</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A14:A15" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A20:A21" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B14:B15" xr:uid="{00000000-0002-0000-0F00-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B20:B21" xr:uid="{00000000-0002-0000-0F00-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4433,10 +4820,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" activeCellId="1" sqref="A4:XFD4 E19"/>
+    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4621,14 +5008,14 @@
       <c r="A11" s="30">
         <v>43466</v>
       </c>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>203</v>
@@ -4638,11 +5025,11 @@
       <c r="A12" s="30">
         <v>43466</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="C12" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E12" s="55" t="s">
         <v>204</v>
@@ -4655,11 +5042,11 @@
       <c r="A13" s="30">
         <v>43466</v>
       </c>
-      <c r="C13" t="s">
-        <v>28</v>
+      <c r="C13" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>204</v>
@@ -4672,11 +5059,11 @@
       <c r="A14" s="30">
         <v>43466</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14" s="55" t="s">
         <v>204</v>
@@ -4689,11 +5076,11 @@
       <c r="A15" s="30">
         <v>43466</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E15" s="55" t="s">
         <v>204</v>
@@ -4706,11 +5093,11 @@
       <c r="A16" s="30">
         <v>43466</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
+      <c r="C16" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E16" s="55" t="s">
         <v>204</v>
@@ -4723,63 +5110,182 @@
       <c r="A17" s="30">
         <v>43466</v>
       </c>
-      <c r="C17" t="s">
-        <v>31</v>
+      <c r="C17" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="8">
+      <c r="A18" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="8">
         <v>45266</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E25" t="s">
         <v>204</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="8">
         <v>45266</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E26" t="s">
         <v>204</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>201</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A18:A19" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A25:A26" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B18:B19" xr:uid="{00000000-0002-0000-1000-000001000000}">
-      <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B25:B26" xr:uid="{00000000-0002-0000-1000-000001000000}">
+      <formula1>IF((DATEDIF(A11,B11,"d")&gt;0),B11)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4790,10 +5296,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A24" activeCellId="1" sqref="A4:XFD4 A24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5063,14 +5569,14 @@
       <c r="A16" s="30">
         <v>43466</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
+      <c r="C16" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>203</v>
@@ -5080,14 +5586,14 @@
       <c r="A17" s="30">
         <v>43466</v>
       </c>
-      <c r="C17" t="s">
-        <v>28</v>
+      <c r="C17" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D17" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>203</v>
@@ -5097,14 +5603,14 @@
       <c r="A18" s="30">
         <v>43466</v>
       </c>
-      <c r="C18" t="s">
-        <v>28</v>
+      <c r="C18" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D18" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>203</v>
@@ -5114,14 +5620,14 @@
       <c r="A19" s="30">
         <v>43466</v>
       </c>
-      <c r="C19" t="s">
-        <v>28</v>
+      <c r="C19" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>203</v>
@@ -5131,14 +5637,14 @@
       <c r="A20" s="30">
         <v>43466</v>
       </c>
-      <c r="C20" t="s">
-        <v>28</v>
+      <c r="C20" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>69</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>203</v>
@@ -5148,14 +5654,14 @@
       <c r="A21" s="30">
         <v>43466</v>
       </c>
-      <c r="C21" t="s">
-        <v>28</v>
+      <c r="C21" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>203</v>
@@ -5165,114 +5671,313 @@
       <c r="A22" s="30">
         <v>43466</v>
       </c>
-      <c r="C22" t="s">
-        <v>31</v>
+      <c r="C22" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D22" t="s">
         <v>52</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8">
+      <c r="A23" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C23" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C24" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C25" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C26" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C27" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="30">
+        <v>43466</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="8">
         <v>45266</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D35" t="s">
         <v>77</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E35" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="30"/>
-      <c r="D24" s="10"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="30"/>
-      <c r="D25" s="10"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="30"/>
-      <c r="D26" s="10"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="30"/>
-      <c r="D27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="30"/>
-      <c r="D28" s="10"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="30"/>
-      <c r="D29" s="10"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="30"/>
-      <c r="D30" s="10"/>
-      <c r="F30" s="10"/>
-    </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="30"/>
-      <c r="D31" s="10"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="30"/>
-      <c r="D32" s="10"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="30"/>
-      <c r="D33" s="10"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="30"/>
-      <c r="D34" s="10"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="30"/>
-      <c r="D35" s="10"/>
-      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="30"/>
       <c r="D36" s="10"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="30"/>
+      <c r="D37" s="10"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="30"/>
+      <c r="D38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="30"/>
+      <c r="D39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="30"/>
+      <c r="D40" s="10"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="30"/>
+      <c r="D41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="30"/>
+      <c r="D42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="30"/>
+      <c r="D43" s="10"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="30"/>
+      <c r="D44" s="10"/>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="30"/>
+      <c r="D45" s="10"/>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="30"/>
+      <c r="D46" s="10"/>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="30"/>
+      <c r="D47" s="10"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="30"/>
+      <c r="D48" s="10"/>
+      <c r="F48" s="10"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A23" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A35" xr:uid="{00000000-0002-0000-1100-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B23" xr:uid="{00000000-0002-0000-1100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B35" xr:uid="{00000000-0002-0000-1100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5390,10 +6095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5503,14 +6208,14 @@
         <v>43466</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
+      <c r="C5" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="112" t="s">
+        <v>267</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>30</v>
+        <v>268</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -5519,19 +6224,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8">
         <v>43466</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -5542,16 +6247,17 @@
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -5560,16 +6266,36 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="J25" s="16"/>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J26" s="16"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5583,7 +6309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -9466,10 +10192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" activeCellId="1" sqref="A4:XFD4 D18"/>
+    <sheetView topLeftCell="G2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9741,8 +10467,8 @@
         <v>43466</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D10" t="s">
         <v>52</v>
@@ -9768,8 +10494,8 @@
         <v>43466</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D11" t="s">
         <v>57</v>
@@ -9795,8 +10521,8 @@
         <v>43466</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="C12" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
@@ -9822,8 +10548,8 @@
         <v>43466</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" t="s">
-        <v>28</v>
+      <c r="C13" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>65</v>
@@ -9849,8 +10575,8 @@
         <v>43466</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>69</v>
@@ -9876,8 +10602,8 @@
         <v>43466</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>73</v>
@@ -9898,13 +10624,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>43466</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -9925,24 +10651,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I17" t="s">
         <v>56</v>
@@ -9951,24 +10678,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>83</v>
+        <v>63</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="I18" t="s">
         <v>56</v>
@@ -9977,19 +10705,173 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1048571" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A18" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A24" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B22" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10322,7 +11204,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" activeCellId="1" sqref="A4:XFD4 C20"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10445,8 +11327,8 @@
         <v>43466</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="C7" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>95</v>
@@ -10463,8 +11345,8 @@
         <v>43466</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" t="s">
-        <v>28</v>
+      <c r="C8" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>97</v>
@@ -10481,8 +11363,8 @@
         <v>43466</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" t="s">
-        <v>28</v>
+      <c r="C9" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>99</v>
@@ -10494,13 +11376,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>43466</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>95</v>
@@ -10514,57 +11396,108 @@
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8">
-        <v>45266</v>
+        <v>43466</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
-        <v>45266</v>
+        <v>43466</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8">
+        <v>45266</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8">
+        <v>45266</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G12">
+      <c r="G15">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G12" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G15" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B12" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10576,10 +11509,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView topLeftCell="B2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" activeCellId="1" sqref="A4:XFD4 C24"/>
+      <selection activeCell="C10" sqref="C10:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10901,8 +11834,8 @@
         <v>43466</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>121</v>
@@ -10928,8 +11861,8 @@
         <v>43466</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>124</v>
@@ -10958,8 +11891,8 @@
         <v>43466</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" t="s">
-        <v>28</v>
+      <c r="C12" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>126</v>
@@ -10988,8 +11921,8 @@
         <v>43466</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" t="s">
-        <v>28</v>
+      <c r="C13" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>128</v>
@@ -11018,8 +11951,8 @@
         <v>43466</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>28</v>
+      <c r="C14" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>130</v>
@@ -11048,8 +11981,8 @@
         <v>43466</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" t="s">
-        <v>28</v>
+      <c r="C15" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>133</v>
@@ -11073,13 +12006,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>43466</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>121</v>
@@ -11097,84 +12030,256 @@
         <v>27</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>135</v>
+        <v>28</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17" t="s">
-        <v>101</v>
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="P17" t="s">
         <v>27</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>136</v>
+        <v>28</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" t="s">
-        <v>103</v>
+        <v>3</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="P18" t="s">
         <v>27</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="P19" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="P20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="P21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P24" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A17:A18" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A23:A24" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G16" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G22" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B16" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B22" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A16" xr:uid="{00000000-0002-0000-0600-000003000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A22" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11186,10 +12291,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView topLeftCell="G25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K41" activeCellId="1" sqref="A4:XFD4 K41"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11963,8 +13068,8 @@
         <v>43466</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" t="s">
-        <v>28</v>
+      <c r="C22" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>121</v>
@@ -11999,8 +13104,8 @@
         <v>43466</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" t="s">
-        <v>28</v>
+      <c r="C23" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>121</v>
@@ -12035,8 +13140,8 @@
         <v>43466</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" t="s">
-        <v>28</v>
+      <c r="C24" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>121</v>
@@ -12071,8 +13176,8 @@
         <v>43466</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" t="s">
-        <v>28</v>
+      <c r="C25" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>121</v>
@@ -12107,8 +13212,8 @@
         <v>43466</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" t="s">
-        <v>28</v>
+      <c r="C26" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>121</v>
@@ -12143,8 +13248,8 @@
         <v>43466</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" t="s">
-        <v>28</v>
+      <c r="C27" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>121</v>
@@ -12179,8 +13284,8 @@
         <v>43466</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" t="s">
-        <v>28</v>
+      <c r="C28" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>130</v>
@@ -12215,8 +13320,8 @@
         <v>43466</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" t="s">
-        <v>28</v>
+      <c r="C29" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>130</v>
@@ -12251,8 +13356,8 @@
         <v>43466</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" t="s">
-        <v>28</v>
+      <c r="C30" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>130</v>
@@ -12287,8 +13392,8 @@
         <v>43466</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" t="s">
-        <v>28</v>
+      <c r="C31" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>130</v>
@@ -12323,8 +13428,8 @@
         <v>43466</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" t="s">
-        <v>28</v>
+      <c r="C32" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>130</v>
@@ -12359,8 +13464,8 @@
         <v>43466</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" t="s">
-        <v>28</v>
+      <c r="C33" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>130</v>
@@ -12395,8 +13500,8 @@
         <v>43466</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" t="s">
-        <v>28</v>
+      <c r="C34" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>133</v>
@@ -12431,8 +13536,8 @@
         <v>43466</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" t="s">
-        <v>28</v>
+      <c r="C35" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>133</v>
@@ -12467,8 +13572,8 @@
         <v>43466</v>
       </c>
       <c r="B36" s="8"/>
-      <c r="C36" t="s">
-        <v>28</v>
+      <c r="C36" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>133</v>
@@ -12503,8 +13608,8 @@
         <v>43466</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" t="s">
-        <v>28</v>
+      <c r="C37" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>133</v>
@@ -12539,8 +13644,8 @@
         <v>43466</v>
       </c>
       <c r="B38" s="8"/>
-      <c r="C38" t="s">
-        <v>28</v>
+      <c r="C38" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>133</v>
@@ -12575,8 +13680,8 @@
         <v>43466</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" t="s">
-        <v>28</v>
+      <c r="C39" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>133</v>
@@ -12606,23 +13711,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B40" s="8"/>
       <c r="C40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" t="s">
-        <v>135</v>
+        <v>28</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40" s="10" t="s">
         <v>56</v>
       </c>
       <c r="I40" t="s">
@@ -12631,58 +13737,705 @@
       <c r="J40" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="K40" t="s">
-        <v>163</v>
+      <c r="K40" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="L40">
         <v>1</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B41" s="8"/>
       <c r="C41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s">
-        <v>136</v>
+        <v>28</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="E41" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="10" t="s">
         <v>56</v>
       </c>
       <c r="I41" t="s">
         <v>158</v>
       </c>
       <c r="J41" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="O41" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="O42" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" t="s">
+        <v>158</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="O43" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" t="s">
+        <v>158</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="O44" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" t="s">
+        <v>158</v>
+      </c>
+      <c r="J45" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K45" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="O45" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I46" t="s">
+        <v>158</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I47" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="O47" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" t="s">
+        <v>158</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I49" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="O49" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50">
+        <v>5</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I50" t="s">
+        <v>158</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" t="s">
+        <v>158</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="O51" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>123</v>
+      </c>
+      <c r="I52" t="s">
+        <v>158</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K52" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" t="s">
+        <v>57</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="H53" t="s">
+        <v>123</v>
+      </c>
+      <c r="I53" t="s">
+        <v>158</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="H54" t="s">
+        <v>123</v>
+      </c>
+      <c r="I54" t="s">
+        <v>158</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="H55" t="s">
+        <v>123</v>
+      </c>
+      <c r="I55" t="s">
+        <v>158</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="H56" t="s">
+        <v>123</v>
+      </c>
+      <c r="I56" t="s">
+        <v>158</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="8">
+        <v>43466</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>123</v>
+      </c>
+      <c r="I57" t="s">
+        <v>158</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="L57">
+        <v>2</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C58" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>56</v>
+      </c>
+      <c r="I58" t="s">
+        <v>158</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K58" t="s">
+        <v>163</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="O58" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="H59" t="s">
+        <v>56</v>
+      </c>
+      <c r="I59" t="s">
+        <v>158</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K59" t="s">
         <v>164</v>
       </c>
-      <c r="L41">
+      <c r="L59">
         <v>2</v>
       </c>
-      <c r="O41" s="10" t="s">
+      <c r="O59" s="10" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A41" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A59" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B39" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B57" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12697,7 +14450,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" activeCellId="1" sqref="A4:XFD4 D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12783,8 +14536,8 @@
         <v>43466</v>
       </c>
       <c r="B5" s="28"/>
-      <c r="C5" t="s">
-        <v>28</v>
+      <c r="C5" s="112" t="s">
+        <v>266</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -12796,13 +14549,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>43466</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
@@ -12816,13 +14569,14 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>45266</v>
-      </c>
+        <v>43466</v>
+      </c>
+      <c r="B7" s="28"/>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>167</v>
@@ -12831,20 +14585,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>45266</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0800-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{300905BA-24E0-1846-9392-80E2F31F0294}">
       <formula1>42736</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F7" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{8B9D558E-6393-BF40-82E3-E47FC4E7FB0F}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>IF((DATEDIF(A7,B7,"d")&gt;0),B7)</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B5" xr:uid="{CB2687BD-26ED-7E45-BA20-C0D7B3045D5D}">
+      <formula1>IF((DATEDIF(A8,B8,"d")&gt;0),B8)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B6:B7" xr:uid="{80FA93BC-C9D0-9C43-96F6-0234558F44A0}">
+      <formula1>IF((DATEDIF(A9,B9,"d")&gt;0),B9)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -12853,23 +14627,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{465E2074-0E4B-014A-BB00-F988ABE854BF}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$9</xm:f>
+            <xm:f>CaseField!$D$10:$D$15</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D4 D6</xm:sqref>
+          <xm:sqref>D7 D4:D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{8FB37F30-20AC-E445-AE8C-C951B9A4191C}">
           <x14:formula1>
             <xm:f>'/users/semenu/library/containers/com.microsoft.excel/data/documents/users\sivakanukollu\github\moj\ccd-data-store-api\src\aat\resources\[ccd_befta_jurisdiction4.xlsx]casefield'!#REF!</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D5</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Change access for CaseType and CaseState from CRU to CU
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D5C55-66FB-BC43-B3F1-4DA54F7E0E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F85F844-8CA4-9B4A-A913-488948DBC9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="33720" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="270">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -884,6 +884,9 @@
   </si>
   <si>
     <t>Create a case of type BEFTA_CASETYPE_NO_READ</t>
+  </si>
+  <si>
+    <t>CU</t>
   </si>
 </sst>
 </file>
@@ -4242,7 +4245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -4340,8 +4343,8 @@
       <c r="D6" t="s">
         <v>204</v>
       </c>
-      <c r="E6" t="s">
-        <v>203</v>
+      <c r="E6" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -4412,7 +4415,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4601,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4619,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4637,7 +4640,7 @@
         <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4655,7 +4658,7 @@
         <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4673,7 +4676,7 @@
         <v>204</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4691,7 +4694,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>203</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5298,7 +5301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change access for CaseType and CaseState from CRU to CU and date from 01/01/2019 to 1/1/19 (without the zero padding)
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F85F844-8CA4-9B4A-A913-488948DBC9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63A230F-91FD-204E-AB4E-7020CCAE45EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -4245,8 +4245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4344,7 +4344,7 @@
         <v>204</v>
       </c>
       <c r="E6" s="112" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -4414,7 +4414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F11" sqref="F11:F15"/>
     </sheetView>
   </sheetViews>
@@ -5020,8 +5020,8 @@
       <c r="E11" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>203</v>
+      <c r="F11" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5037,8 +5037,8 @@
       <c r="E12" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>203</v>
+      <c r="F12" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5054,8 +5054,8 @@
       <c r="E13" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>203</v>
+      <c r="F13" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5071,8 +5071,8 @@
       <c r="E14" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>203</v>
+      <c r="F14" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5088,8 +5088,8 @@
       <c r="E15" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>203</v>
+      <c r="F15" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5105,8 +5105,8 @@
       <c r="E16" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>203</v>
+      <c r="F16" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5122,8 +5122,8 @@
       <c r="E17" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>203</v>
+      <c r="F17" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5302,7 +5302,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F22" sqref="F22:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5683,8 +5683,8 @@
       <c r="E22" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>203</v>
+      <c r="F22" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5700,8 +5700,8 @@
       <c r="E23" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>203</v>
+      <c r="F23" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5717,8 +5717,8 @@
       <c r="E24" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>203</v>
+      <c r="F24" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5734,8 +5734,8 @@
       <c r="E25" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>203</v>
+      <c r="F25" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5751,8 +5751,8 @@
       <c r="E26" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>203</v>
+      <c r="F26" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5768,8 +5768,8 @@
       <c r="E27" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>203</v>
+      <c r="F27" s="112" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
To fix inconsistency in FT testing for ccd-data-store FT-1025 S-1025.3
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63A230F-91FD-204E-AB4E-7020CCAE45EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B4637-C7EE-054B-B1DC-C4A009B8DA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4415,7 +4415,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F15"/>
+      <selection activeCell="F10" sqref="F10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4622,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4640,7 +4640,7 @@
         <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4658,7 +4658,7 @@
         <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,7 +4676,7 @@
         <v>204</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4694,7 +4694,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ccd 5329 unassigned acknowledging assigning cases ccd cnp rdm5118 (#96)
* Modified CCD_CNP_RDM5118.xlsx to have for case_type ATT_AUTH_15, CallbackGetCaseUrl" : "${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/case_type/fe-functional-test/callback_get_case" instead of 'http://host.docker.internal:5555/case_type/fe-functional'-test/callback_get_case

* To fix inconsistency in FT testing for ccd-data-store FT-1025 S-1025.3
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63A230F-91FD-204E-AB4E-7020CCAE45EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B4637-C7EE-054B-B1DC-C4A009B8DA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4415,7 +4415,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F15"/>
+      <selection activeCell="F10" sqref="F10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4622,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4640,7 +4640,7 @@
         <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4658,7 +4658,7 @@
         <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,7 +4676,7 @@
         <v>204</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4694,7 +4694,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Changes to Fix FT-1025, S-1025.3 failing
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63A230F-91FD-204E-AB4E-7020CCAE45EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D425F64-9D34-8040-8883-118AC20A067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4415,7 +4415,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F15"/>
+      <selection activeCell="F10" sqref="F10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4622,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4640,7 +4640,7 @@
         <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4658,7 +4658,7 @@
         <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,7 +4676,7 @@
         <v>204</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4694,7 +4694,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Changes to Fix FT-1025, S-1025.3 failing (#100)
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_BEFTA_JURISDICTION1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilapatel/Documents/Work/repos/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63A230F-91FD-204E-AB4E-7020CCAE45EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D425F64-9D34-8040-8883-118AC20A067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30220" yWindow="1400" windowWidth="30220" windowHeight="19860" tabRatio="500" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4415,7 +4415,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F15"/>
+      <selection activeCell="F10" sqref="F10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4604,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4622,7 +4622,7 @@
         <v>202</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4640,7 +4640,7 @@
         <v>202</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4658,7 +4658,7 @@
         <v>204</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4676,7 +4676,7 @@
         <v>204</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4694,7 +4694,7 @@
         <v>204</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>